<commit_message>
Conclusão da tabela de custos
</commit_message>
<xml_diff>
--- a/03-CRONOGRAMA.xlsx
+++ b/03-CRONOGRAMA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafael.j.dos.santos\Desktop\UNINASSAU\6 PERIODO\PROJETO DE ANALISE\DOCUMENTAÇÃO PARA O PROJETO\DOCUMENTOS\proj-grupo5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.da.cunha.costa\Desktop\Projeto Rei do Cangaço - documentação\proj-grupo5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF15BE1-EC1B-4041-8878-1F43A6426C7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A93970-4A45-4641-9CBF-F725A5334177}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{070E63A1-769A-4DD3-A3A8-D30620403D05}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{070E63A1-769A-4DD3-A3A8-D30620403D05}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma de Atividades" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>Tarefa</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>30, 00</t>
+  </si>
+  <si>
+    <t>DESENVOLVEDOR BANCO</t>
   </si>
 </sst>
 </file>
@@ -239,7 +242,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -293,6 +296,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -320,7 +345,7 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1">
@@ -356,6 +381,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Activity" xfId="3" xr:uid="{57776DFF-96F3-4A8A-BD32-B17F1F683B7E}"/>
@@ -1618,22 +1652,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{945DCC05-F2FC-492E-8062-1938DAA8C20E}">
   <dimension ref="B1:N29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" style="1"/>
-    <col min="2" max="2" width="30.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.77734375" style="1"/>
+    <col min="1" max="1" width="8.81640625" style="1"/>
+    <col min="2" max="2" width="30.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -1648,7 +1682,7 @@
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
     </row>
-    <row r="2" spans="2:14" ht="24.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:14" ht="25" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1665,7 +1699,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="4" spans="2:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:14" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B4" s="5" t="s">
         <v>0</v>
       </c>
@@ -1688,7 +1722,7 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="2:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:14" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B5" s="8" t="s">
         <v>5</v>
       </c>
@@ -1712,7 +1746,7 @@
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
     </row>
-    <row r="6" spans="2:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:14" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B6" s="8" t="s">
         <v>6</v>
       </c>
@@ -1736,7 +1770,7 @@
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
     </row>
-    <row r="7" spans="2:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:14" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B7" s="8" t="s">
         <v>7</v>
       </c>
@@ -1760,7 +1794,7 @@
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
     </row>
-    <row r="8" spans="2:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:14" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B8" s="8" t="s">
         <v>8</v>
       </c>
@@ -1784,7 +1818,7 @@
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
     </row>
-    <row r="9" spans="2:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:14" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B9" s="11" t="s">
         <v>12</v>
       </c>
@@ -1808,7 +1842,7 @@
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
     </row>
-    <row r="10" spans="2:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:14" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B10" s="11" t="s">
         <v>9</v>
       </c>
@@ -1832,7 +1866,7 @@
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
     </row>
-    <row r="11" spans="2:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:14" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B11" s="8" t="s">
         <v>10</v>
       </c>
@@ -1856,7 +1890,7 @@
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
     </row>
-    <row r="12" spans="2:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:14" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B12" s="8" t="s">
         <v>11</v>
       </c>
@@ -1880,26 +1914,26 @@
       <c r="M12" s="8"/>
       <c r="N12" s="8"/>
     </row>
-    <row r="15" spans="2:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:14" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B15" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C15" s="7"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B17" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="F17" s="17"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B18" s="13" t="s">
         <v>14</v>
       </c>
@@ -1912,17 +1946,17 @@
       <c r="E18" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F18" s="13" t="s">
+      <c r="F18" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G18" s="19"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B19" s="13" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>18</v>
@@ -1930,14 +1964,18 @@
       <c r="D19" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E19" s="13">
+        <v>15</v>
+      </c>
+      <c r="F19" s="18">
+        <v>450</v>
+      </c>
+      <c r="G19" s="19"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B20" s="13" t="s">
         <v>27</v>
       </c>
@@ -1947,14 +1985,18 @@
       <c r="D20" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E20" s="13">
+        <v>90</v>
+      </c>
+      <c r="F20" s="18">
+        <v>2700</v>
+      </c>
+      <c r="G20" s="19"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B21" s="13" t="s">
         <v>25</v>
       </c>
@@ -1964,14 +2006,18 @@
       <c r="D21" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E21" s="13">
+        <v>90</v>
+      </c>
+      <c r="F21" s="18">
+        <v>2700</v>
+      </c>
+      <c r="G21" s="19"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B22" s="13" t="s">
         <v>26</v>
       </c>
@@ -1981,44 +2027,56 @@
       <c r="D22" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E22" s="13">
+        <v>45</v>
+      </c>
+      <c r="F22" s="18">
+        <v>1350</v>
+      </c>
+      <c r="G22" s="19"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B23" s="13" t="s">
         <v>15</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="13"/>
+      <c r="D23" s="15">
+        <v>336.68</v>
+      </c>
       <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="F23" s="17">
+        <v>336.68</v>
+      </c>
+      <c r="G23" s="19"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B24" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C24" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="13"/>
+      <c r="D24" s="16">
+        <v>336.68</v>
+      </c>
       <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="F24" s="17">
+        <v>336.68</v>
+      </c>
+      <c r="G24" s="19"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
@@ -2028,7 +2086,7 @@
       <c r="I25" s="14"/>
       <c r="J25" s="14"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C26" s="14"/>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
@@ -2038,7 +2096,7 @@
       <c r="I26" s="14"/>
       <c r="J26" s="14"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
@@ -2049,7 +2107,7 @@
       <c r="I27" s="14"/>
       <c r="J27" s="14"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B28" s="14" t="s">
         <v>22</v>
       </c>
@@ -2062,7 +2120,7 @@
       <c r="I28" s="14"/>
       <c r="J28" s="14"/>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B29" s="14" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Tabela de custos concluída
</commit_message>
<xml_diff>
--- a/03-CRONOGRAMA.xlsx
+++ b/03-CRONOGRAMA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.da.cunha.costa\Desktop\Projeto Rei do Cangaço - documentação\proj-grupo5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A93970-4A45-4641-9CBF-F725A5334177}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8FA2F7-B20D-42B5-B7A9-0101A53F7993}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{070E63A1-769A-4DD3-A3A8-D30620403D05}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>Tarefa</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>DESENVOLVEDOR BANCO</t>
+  </si>
+  <si>
+    <t>TOTAL CUSTOS</t>
   </si>
 </sst>
 </file>
@@ -242,7 +245,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -318,6 +321,58 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -345,7 +400,7 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1">
@@ -390,6 +445,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Activity" xfId="3" xr:uid="{57776DFF-96F3-4A8A-BD32-B17F1F683B7E}"/>
@@ -1652,8 +1711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{945DCC05-F2FC-492E-8062-1938DAA8C20E}">
   <dimension ref="B1:N29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2057,7 +2116,7 @@
       <c r="I23" s="14"/>
       <c r="J23" s="14"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B24" s="13" t="s">
         <v>16</v>
       </c>
@@ -2067,8 +2126,8 @@
       <c r="D24" s="16">
         <v>336.68</v>
       </c>
-      <c r="E24" s="13"/>
-      <c r="F24" s="17">
+      <c r="E24" s="20"/>
+      <c r="F24" s="21">
         <v>336.68</v>
       </c>
       <c r="G24" s="19"/>
@@ -2076,11 +2135,16 @@
       <c r="I24" s="14"/>
       <c r="J24" s="14"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
+      <c r="E25" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" s="23">
+        <f>SUM(F19:F24)</f>
+        <v>7873.3600000000006</v>
+      </c>
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
       <c r="I25" s="14"/>

</xml_diff>

<commit_message>
criando o documento de tabelemanto de custos
</commit_message>
<xml_diff>
--- a/03-CRONOGRAMA.xlsx
+++ b/03-CRONOGRAMA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.da.cunha.costa\Desktop\Projeto Rei do Cangaço - documentação\proj-grupo5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafael.j.dos.santos\Desktop\UNINASSAU\6 PERIODO\PROJETO DE ANALISE\DOCUMENTAÇÃO PARA O PROJETO\DOCUMENTOS\proj-grupo5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9577701-B771-4184-AD9E-20A425AFB7FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B345F8-A458-4396-8A86-235A683473B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{070E63A1-769A-4DD3-A3A8-D30620403D05}"/>
+    <workbookView xWindow="624" yWindow="600" windowWidth="22416" windowHeight="11760" xr2:uid="{070E63A1-769A-4DD3-A3A8-D30620403D05}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma de Atividades" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Tarefa</t>
   </si>
@@ -72,63 +72,6 @@
   </si>
   <si>
     <t>Criar Banco de dados</t>
-  </si>
-  <si>
-    <t>CUSTOS</t>
-  </si>
-  <si>
-    <t>FUNÇAO</t>
-  </si>
-  <si>
-    <t>HOSPEDAGEM WEB BANCO</t>
-  </si>
-  <si>
-    <t>HOSPEDAGEM WEB SISTEMA</t>
-  </si>
-  <si>
-    <t>VINCULO</t>
-  </si>
-  <si>
-    <t>PESSOA FISICA</t>
-  </si>
-  <si>
-    <t>CUSTO/HORA</t>
-  </si>
-  <si>
-    <t>TOTAL DE HORAS</t>
-  </si>
-  <si>
-    <t>TOTAL R$</t>
-  </si>
-  <si>
-    <t>OBS: NOS CUSTOS SE FOR UM FUNCIONARIO ALEM DO SALARIO TEM Q COLOCAR OS DEMAIS VALORES QUE VAI SER NECESSARIO PAGAR AO TRABALHADOR DE UMA FORMA GERAL</t>
-  </si>
-  <si>
-    <t>OU SEJA, CUSTO DE UM FUNCIONARIO LIQUIDO PARA UMA EMPRESA, TEM NA INTERNET A CALCULADORA - CALCULADOR.COM.BR</t>
-  </si>
-  <si>
-    <t>TABELA DE CUSTOS</t>
-  </si>
-  <si>
-    <t>DESENVOLVEDOR FRONT END</t>
-  </si>
-  <si>
-    <t>TESTER</t>
-  </si>
-  <si>
-    <t>DESENVOLVEDOR BACK END</t>
-  </si>
-  <si>
-    <t>SERVICE</t>
-  </si>
-  <si>
-    <t>30, 00</t>
-  </si>
-  <si>
-    <t>DESENVOLVEDOR BANCO</t>
-  </si>
-  <si>
-    <t>TOTAL CUSTOS</t>
   </si>
 </sst>
 </file>
@@ -231,7 +174,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -244,14 +187,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="11">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -290,95 +227,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -406,7 +254,7 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1">
@@ -424,7 +272,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -440,21 +287,15 @@
     <xf numFmtId="14" fontId="12" fillId="0" borderId="3" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Activity" xfId="3" xr:uid="{57776DFF-96F3-4A8A-BD32-B17F1F683B7E}"/>
@@ -1715,24 +1556,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{945DCC05-F2FC-492E-8062-1938DAA8C20E}">
-  <dimension ref="B1:N29"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="1"/>
-    <col min="2" max="2" width="30.81640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.81640625" style="1"/>
+    <col min="1" max="1" width="8.77734375" style="1"/>
+    <col min="2" max="2" width="30.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -1747,7 +1588,7 @@
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
     </row>
-    <row r="2" spans="2:14" ht="25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="24.6" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1764,7 +1605,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="4" spans="2:14" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>0</v>
       </c>
@@ -1787,413 +1628,371 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="2:14" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B5" s="8" t="s">
+    <row r="5" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="11">
         <v>44111</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="9">
         <v>2</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="8">
         <f t="shared" ref="E5:E12" si="0">C5+D5</f>
         <v>44113</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-    </row>
-    <row r="6" spans="2:14" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B6" s="8" t="s">
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+    </row>
+    <row r="6" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <v>44112</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>1</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <f t="shared" si="0"/>
         <v>44113</v>
       </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-    </row>
-    <row r="7" spans="2:14" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B7" s="8" t="s">
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+    </row>
+    <row r="7" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <v>44112</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <v>2</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="8">
         <f t="shared" si="0"/>
         <v>44114</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-    </row>
-    <row r="8" spans="2:14" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B8" s="8" t="s">
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+    </row>
+    <row r="8" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="8">
         <v>44112</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>2</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="8">
         <f t="shared" si="0"/>
         <v>44114</v>
       </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-    </row>
-    <row r="9" spans="2:14" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B9" s="11" t="s">
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+    </row>
+    <row r="9" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="8">
         <v>44116</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="9">
         <v>2</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="8">
         <f t="shared" si="0"/>
         <v>44118</v>
       </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-    </row>
-    <row r="10" spans="2:14" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B10" s="11" t="s">
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+    </row>
+    <row r="10" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B10" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <v>44116</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="9">
         <v>10</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="8">
         <f t="shared" si="0"/>
         <v>44126</v>
       </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-    </row>
-    <row r="11" spans="2:14" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B11" s="8" t="s">
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+    </row>
+    <row r="11" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="8">
         <v>44119</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="9">
         <v>20</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="8">
         <f t="shared" si="0"/>
         <v>44139</v>
       </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-    </row>
-    <row r="12" spans="2:14" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B12" s="8" t="s">
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+    </row>
+    <row r="12" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="8">
         <v>44124</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="9">
         <v>5</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="8">
         <f t="shared" si="0"/>
         <v>44129</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-    </row>
-    <row r="15" spans="2:14" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B15" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="7"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B17" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B18" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="G18" s="19"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B19" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E19" s="13">
-        <v>15</v>
-      </c>
-      <c r="F19" s="18">
-        <v>450</v>
-      </c>
-      <c r="G19" s="19"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B20" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E20" s="13">
-        <v>90</v>
-      </c>
-      <c r="F20" s="18">
-        <v>2700</v>
-      </c>
-      <c r="G20" s="19"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B21" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E21" s="13">
-        <v>90</v>
-      </c>
-      <c r="F21" s="18">
-        <v>2700</v>
-      </c>
-      <c r="G21" s="19"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B22" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E22" s="13">
-        <v>45</v>
-      </c>
-      <c r="F22" s="18">
-        <v>1350</v>
-      </c>
-      <c r="G22" s="19"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B23" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23" s="15">
-        <v>336.68</v>
-      </c>
-      <c r="E23" s="13"/>
-      <c r="F23" s="17">
-        <v>336.68</v>
-      </c>
-      <c r="G23" s="19"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-    </row>
-    <row r="24" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="16">
-        <v>336.68</v>
-      </c>
-      <c r="E24" s="20"/>
-      <c r="F24" s="21">
-        <v>336.68</v>
-      </c>
-      <c r="G24" s="19"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-    </row>
-    <row r="25" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="F25" s="23">
-        <f>SUM(F19:F24)</f>
-        <v>7873.3600000000006</v>
-      </c>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B28" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B29" s="14" t="s">
-        <v>23</v>
-      </c>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+    </row>
+    <row r="15" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="12"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>